<commit_message>
20-Jan 2025 - Final
</commit_message>
<xml_diff>
--- a/TestData/T2057_ContactDetailsPage_ActivitiesEdit_AddNewCompany.xlsx
+++ b/TestData/T2057_ContactDetailsPage_ActivitiesEdit_AddNewCompany.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDC2C05-124D-47C0-AAD8-CBE87E2EAF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242A06E6-2CC2-429C-A7C2-0DDB7B394F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -29,80 +29,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
-  <si>
-    <t>ActivityType</t>
-  </si>
-  <si>
-    <t>ActivitySubject</t>
-  </si>
-  <si>
-    <t>Activity Heading</t>
-  </si>
-  <si>
-    <t>Activity Details</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>CompanyName</t>
   </si>
   <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
     <t>Meeting</t>
   </si>
   <si>
-    <t>StdUser</t>
-  </si>
-  <si>
-    <t>Please mark the "No External Contact" checkbox if you wish not to include an primary external attendee on this activity</t>
-  </si>
-  <si>
-    <t>No External Contact Error</t>
-  </si>
-  <si>
-    <t>Lookup Company</t>
-  </si>
-  <si>
-    <t>ActivityCompany</t>
-  </si>
-  <si>
-    <t>Conference 01</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>ContactTypesValue</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>(541) 754-3010</t>
-  </si>
-  <si>
     <t>External Contact</t>
   </si>
   <si>
-    <t>jimmyContact</t>
-  </si>
-  <si>
-    <t>testJimmy@email.com</t>
-  </si>
-  <si>
     <t>ContactType</t>
   </si>
   <si>
-    <t>Lookup Contact</t>
-  </si>
-  <si>
     <t>Test External</t>
   </si>
   <si>
@@ -118,16 +58,55 @@
     <t>Operating Company</t>
   </si>
   <si>
-    <t>Internal Notes</t>
-  </si>
-  <si>
-    <t>Testing Notes</t>
-  </si>
-  <si>
-    <t>Updated Internal Notes</t>
-  </si>
-  <si>
-    <t>Ayati Arvind</t>
+    <t>Thomas Bailey</t>
+  </si>
+  <si>
+    <t>CF Financial User</t>
+  </si>
+  <si>
+    <t>StandardTestCompany</t>
+  </si>
+  <si>
+    <t>ContactName</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>IndustryGroup</t>
+  </si>
+  <si>
+    <t>ProductType</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>MeetingNotes</t>
+  </si>
+  <si>
+    <t>ExtAttendee</t>
+  </si>
+  <si>
+    <t>BUS - Business Services</t>
+  </si>
+  <si>
+    <t>Activist Advisory</t>
+  </si>
+  <si>
+    <t>Meeting Notes 1</t>
+  </si>
+  <si>
+    <t>Test Activity with new company</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>United States</t>
   </si>
 </sst>
 </file>
@@ -177,7 +156,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,12 +453,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -488,81 +469,67 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
+      <c r="C2" t="s">
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -573,6 +540,47 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -581,88 +589,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -684,12 +628,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>